<commit_message>
updates doc et bom
</commit_message>
<xml_diff>
--- a/BOM (Autosaved).xlsx
+++ b/BOM (Autosaved).xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="5900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15340" windowHeight="5900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fournitures" sheetId="1" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>Elément</t>
   </si>
@@ -449,6 +448,15 @@
   </si>
   <si>
     <t>https://www.mouser.fr/ProductDetail/571-2-1571552-4</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Resistor-Networks-Arrays_FH-Guangdong-Fenghua-Advanced-Tech-A09-471JP_C51158.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/IC-Sockets_CONNFLY-Elec-DS1001-01-16BT1NSF6X-JKB_C72130.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -536,8 +544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G45" totalsRowShown="0">
-  <autoFilter ref="A1:G45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G47" totalsRowShown="0">
+  <autoFilter ref="A1:G47"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Elément"/>
     <tableColumn id="2" name="Nombre"/>
@@ -833,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,7 +854,8 @@
     <col min="3" max="3" width="13.90625" customWidth="1"/>
     <col min="4" max="4" width="44.7265625" customWidth="1"/>
     <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" customWidth="1"/>
+    <col min="6" max="6" width="33.7265625" customWidth="1"/>
+    <col min="7" max="7" width="35.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -953,7 +962,7 @@
       <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -974,7 +983,7 @@
       <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -983,102 +992,106 @@
         <v>139</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>1.17</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D7">
-        <v>23.4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>140</v>
+        <v>1.44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>5.8999999999999997E-2</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="2">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>1.17</v>
       </c>
       <c r="D8">
-        <v>0.59</v>
+        <v>23.4</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
       <c r="C9">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>4.0999999999999995E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D9">
-        <v>0.41</v>
+        <v>0.59</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>2.8000000000000004E-2</v>
+        <v>4.0999999999999995E-2</v>
       </c>
       <c r="D10">
-        <v>0.28000000000000003</v>
+        <v>0.41</v>
       </c>
       <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" t="s">
-        <v>51</v>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>16</v>
+        <v>2.8000000000000004E-2</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1090,118 +1103,121 @@
       </c>
       <c r="C12">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>4.99</v>
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>4.99</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>5.1000000000000004E-2</v>
+        <v>4.99</v>
       </c>
       <c r="D13">
-        <v>0.51</v>
+        <v>4.99</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>8.24</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="D14">
-        <v>8.24</v>
+        <v>0.51</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>3.31</v>
+        <v>8.24</v>
       </c>
       <c r="D15">
-        <v>3.31</v>
+        <v>8.24</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.65</v>
+        <v>3.31</v>
       </c>
       <c r="D16">
-        <v>6.5</v>
+        <v>3.31</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0</v>
+        <v>0.65</v>
+      </c>
+      <c r="D17">
+        <v>6.5</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1209,20 +1225,17 @@
         <v>11</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>1.448</v>
-      </c>
-      <c r="D18">
-        <v>7.24</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1230,586 +1243,620 @@
         <v>11</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.36899999999999999</v>
+        <v>1.448</v>
       </c>
       <c r="D19">
-        <v>3.69</v>
+        <v>7.24</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.55999999999999994</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="D20">
-        <v>5.6</v>
+        <v>3.69</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.49000000000000005</v>
+        <v>0.55999999999999994</v>
       </c>
       <c r="D21">
-        <v>4.9000000000000004</v>
+        <v>5.6</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>1.1220000000000001E-2</v>
+        <v>0.49000000000000005</v>
       </c>
       <c r="D22">
-        <v>5.61</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C23">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>1.5866666666666664E-2</v>
+        <v>1.1220000000000001E-2</v>
       </c>
       <c r="D23">
-        <v>4.76</v>
+        <v>5.61</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="C24">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.2</v>
+        <v>1.5866666666666664E-2</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>4.76</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>9.1799999999999993E-2</v>
+        <v>0.2</v>
       </c>
       <c r="D25">
-        <v>9.18</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.13300000000000001</v>
+        <v>9.1799999999999993E-2</v>
       </c>
       <c r="D26">
-        <v>1.33</v>
+        <v>9.18</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>10</v>
       </c>
       <c r="C27">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>1.59</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="D27">
-        <v>15.9</v>
+        <v>1.33</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.92699999999999994</v>
+        <v>1.59</v>
       </c>
       <c r="D28">
-        <v>9.27</v>
+        <v>15.9</v>
       </c>
       <c r="E28" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
       <c r="C29">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.23100000000000001</v>
+        <v>0.92699999999999994</v>
       </c>
       <c r="D29">
-        <v>2.31</v>
+        <v>9.27</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.53200000000000003</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="D30">
-        <v>2.66</v>
+        <v>2.31</v>
       </c>
       <c r="E30" t="s">
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
       <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31" s="2">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.14399999999999999</v>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>0.53200000000000003</v>
       </c>
       <c r="D31">
-        <v>1.44</v>
+        <v>2.66</v>
       </c>
       <c r="E31" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>116</v>
-      </c>
-      <c r="G31" s="2"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B32">
         <v>10</v>
       </c>
       <c r="C32" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.11100000000000002</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D32">
-        <v>1.1100000000000001</v>
+        <v>1.44</v>
       </c>
       <c r="E32" t="s">
         <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B33">
         <v>10</v>
       </c>
       <c r="C33" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.13500000000000001</v>
+        <v>0.11100000000000002</v>
       </c>
       <c r="D33">
-        <v>1.35</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E33" t="s">
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B34">
         <v>10</v>
       </c>
       <c r="C34" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.33799999999999997</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D34">
-        <v>3.38</v>
+        <v>1.35</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C35" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>9.8000000000000004E-2</v>
+        <v>0.33799999999999997</v>
       </c>
       <c r="D35">
-        <v>0.49</v>
+        <v>3.38</v>
       </c>
       <c r="E35" t="s">
         <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.13600000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="C36" s="2">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="D36">
-        <v>1.36</v>
+        <v>0.49</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <v>10</v>
       </c>
       <c r="C37">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.32</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="D37">
-        <v>3.2</v>
+        <v>1.36</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>0.32</v>
+      </c>
+      <c r="D38">
+        <v>3.2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>5</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f>0.55*5</f>
         <v>2.75</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>57</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>63</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>5</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
         <v>0.54</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f>0.54*5</f>
         <v>2.7</v>
       </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40">
-        <v>10</v>
-      </c>
-      <c r="C40">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.34700000000000003</v>
-      </c>
-      <c r="D40">
-        <v>3.47</v>
-      </c>
       <c r="E40" t="s">
         <v>57</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>0.34700000000000003</v>
+      </c>
+      <c r="D41">
+        <v>3.47</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
         <v>0.75</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <f>5*0.75</f>
         <v>3.75</v>
       </c>
-      <c r="E41" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42">
-        <v>100</v>
-      </c>
-      <c r="C42">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="D42">
-        <v>2.1</v>
-      </c>
       <c r="E42" t="s">
         <v>57</v>
       </c>
       <c r="F42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C43">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>7.2999999999999995E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D43">
-        <v>3.65</v>
+        <v>2.1</v>
       </c>
       <c r="E43" t="s">
         <v>57</v>
       </c>
       <c r="F43" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="B44">
-        <v>20</v>
-      </c>
-      <c r="C44" s="2">
-        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
-        <v>0.44850000000000001</v>
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="D44">
-        <v>8.9700000000000006</v>
+        <v>3.65</v>
       </c>
       <c r="E44" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G44" s="2"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45" s="2">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>0.44850000000000001</v>
+      </c>
+      <c r="D45">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="E45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F45" t="s">
+        <v>126</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>110</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>10</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C46" s="2">
         <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
         <v>0.44600000000000001</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <f>3.8+0.66</f>
         <v>4.46</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>41</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>127</v>
       </c>
-      <c r="G45" s="2"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="2" t="e">
+        <f>Table2[[#This Row],[Prix total]]/Table2[[#This Row],[Nombre]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F12" r:id="rId1"/>
+    <hyperlink ref="F13" r:id="rId1"/>
+    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1818,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f>Fournitures!C14</f>
+        <f>Fournitures!C15</f>
         <v>8.24</v>
       </c>
       <c r="D5">
@@ -1925,7 +1972,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <f>Fournitures!C44</f>
+        <f>Fournitures!C45</f>
         <v>0.44850000000000001</v>
       </c>
       <c r="D6">
@@ -1973,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <f>Fournitures!C13</f>
+        <f>Fournitures!C14</f>
         <v>5.1000000000000004E-2</v>
       </c>
       <c r="D8">
@@ -1989,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <f>Fournitures!C45</f>
+        <f>Fournitures!C46</f>
         <v>0.44600000000000001</v>
       </c>
       <c r="D9">
@@ -2023,7 +2070,7 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <f>Fournitures!C24</f>
+        <f>Fournitures!C25</f>
         <v>0.2</v>
       </c>
       <c r="D11">
@@ -2075,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <f>Fournitures!C27</f>
+        <f>Fournitures!C28</f>
         <v>1.59</v>
       </c>
       <c r="D14">
@@ -2124,7 +2171,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <f>Fournitures!C15</f>
+        <f>Fournitures!C16</f>
         <v>3.31</v>
       </c>
       <c r="D18">
@@ -2158,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <f>Fournitures!C12</f>
+        <f>Fournitures!C13</f>
         <v>4.99</v>
       </c>
       <c r="D20">
@@ -2174,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <f>Fournitures!C44</f>
+        <f>Fournitures!C45</f>
         <v>0.44850000000000001</v>
       </c>
       <c r="D21">
@@ -2190,7 +2237,7 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <f>Fournitures!C44</f>
+        <f>Fournitures!C45</f>
         <v>0.44850000000000001</v>
       </c>
       <c r="D22">
@@ -2221,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <f>Fournitures!C29</f>
+        <f>Fournitures!C30</f>
         <v>0.23100000000000001</v>
       </c>
       <c r="D25">
@@ -2237,7 +2284,7 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>Fournitures!C33</f>
+        <f>Fournitures!C34</f>
         <v>0.13500000000000001</v>
       </c>
       <c r="D26">
@@ -2253,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <f>Fournitures!C42</f>
+        <f>Fournitures!C43</f>
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D27">
@@ -2269,7 +2316,7 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <f>Fournitures!C34</f>
+        <f>Fournitures!C35</f>
         <v>0.33799999999999997</v>
       </c>
       <c r="D28">
@@ -2285,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <f>Fournitures!C31</f>
+        <f>Fournitures!C32</f>
         <v>0.14399999999999999</v>
       </c>
       <c r="D29" s="2">
@@ -2316,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <f>Fournitures!C38</f>
+        <f>Fournitures!C39</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="D32">
@@ -2332,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <f>Fournitures!C39</f>
+        <f>Fournitures!C40</f>
         <v>0.54</v>
       </c>
       <c r="D33">
@@ -2348,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <f>Fournitures!C41</f>
+        <f>Fournitures!C42</f>
         <v>0.75</v>
       </c>
       <c r="D34">
@@ -2364,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="C35">
-        <f>Fournitures!C40</f>
+        <f>Fournitures!C41</f>
         <v>0.34700000000000003</v>
       </c>
       <c r="D35">
@@ -2380,7 +2427,7 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <f>Fournitures!C42</f>
+        <f>Fournitures!C43</f>
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D36">
@@ -2396,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <f>Fournitures!C43</f>
+        <f>Fournitures!C44</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="D37">
@@ -2412,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <f>Fournitures!C8</f>
+        <f>Fournitures!C9</f>
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="D38">
@@ -2428,7 +2475,7 @@
         <v>2</v>
       </c>
       <c r="C39">
-        <f>Fournitures!C9</f>
+        <f>Fournitures!C10</f>
         <v>4.0999999999999995E-2</v>
       </c>
       <c r="D39">
@@ -2444,7 +2491,7 @@
         <v>8</v>
       </c>
       <c r="C40">
-        <f>Fournitures!C23</f>
+        <f>Fournitures!C24</f>
         <v>1.5866666666666664E-2</v>
       </c>
       <c r="D40">
@@ -2460,7 +2507,7 @@
         <v>16</v>
       </c>
       <c r="C41">
-        <f>Fournitures!C23</f>
+        <f>Fournitures!C24</f>
         <v>1.5866666666666664E-2</v>
       </c>
       <c r="D41">
@@ -2476,7 +2523,7 @@
         <v>16</v>
       </c>
       <c r="C42">
-        <f>Fournitures!C23</f>
+        <f>Fournitures!C24</f>
         <v>1.5866666666666664E-2</v>
       </c>
       <c r="D42">
@@ -2492,7 +2539,7 @@
         <v>16</v>
       </c>
       <c r="C43">
-        <f>Fournitures!C19</f>
+        <f>Fournitures!C20</f>
         <v>0.36899999999999999</v>
       </c>
       <c r="D43">
@@ -2508,7 +2555,7 @@
         <v>4</v>
       </c>
       <c r="C44">
-        <f>Fournitures!C21</f>
+        <f>Fournitures!C22</f>
         <v>0.49000000000000005</v>
       </c>
       <c r="D44">
@@ -2524,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <f>Fournitures!C10</f>
+        <f>Fournitures!C11</f>
         <v>2.8000000000000004E-2</v>
       </c>
       <c r="D45">
@@ -2540,7 +2587,7 @@
         <v>4</v>
       </c>
       <c r="C46">
-        <f>Fournitures!C25</f>
+        <f>Fournitures!C26</f>
         <v>9.1799999999999993E-2</v>
       </c>
       <c r="D46">
@@ -2556,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="C47">
-        <f>Fournitures!C26</f>
+        <f>Fournitures!C27</f>
         <v>0.13300000000000001</v>
       </c>
       <c r="D47">
@@ -2572,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <f>Fournitures!C33</f>
+        <f>Fournitures!C34</f>
         <v>0.13500000000000001</v>
       </c>
       <c r="D48">

</xml_diff>